<commit_message>
Created a DataProvider Util for the Excel Data taht is used for CreateJobAPIExcelDataDrivenTest
And added the changes to datadriven xml file too.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/PhoenixTestData.xlsx
+++ b/src/test/resources/testdata/PhoenixTestData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27040" windowHeight="12500"/>
+    <workbookView windowWidth="27040" windowHeight="12500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="4" r:id="rId1"/>
+    <sheet name="CreateJobTestData" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="58">
   <si>
     <t>username</t>
   </si>
@@ -42,6 +43,165 @@
   </si>
   <si>
     <t>iameng</t>
+  </si>
+  <si>
+    <t>mst_service_location_id</t>
+  </si>
+  <si>
+    <t>mst_platform_id</t>
+  </si>
+  <si>
+    <t>mst_warrenty_status_id</t>
+  </si>
+  <si>
+    <t>mst_oem_id</t>
+  </si>
+  <si>
+    <t>customer__first_name</t>
+  </si>
+  <si>
+    <t>customer__last_name</t>
+  </si>
+  <si>
+    <t>customer__mobile_number</t>
+  </si>
+  <si>
+    <t>customer__mobile_number_alt</t>
+  </si>
+  <si>
+    <t>customer__email_id</t>
+  </si>
+  <si>
+    <t>customer__email_id_alt</t>
+  </si>
+  <si>
+    <t>customer_address__flat_number</t>
+  </si>
+  <si>
+    <t>customer_address__apartment_name</t>
+  </si>
+  <si>
+    <t>customer_address__street_name</t>
+  </si>
+  <si>
+    <t>customer_address__landmark</t>
+  </si>
+  <si>
+    <t>customer_address__area</t>
+  </si>
+  <si>
+    <t>customer_address__pincode</t>
+  </si>
+  <si>
+    <t>customer_address__country</t>
+  </si>
+  <si>
+    <t>customer_address__state</t>
+  </si>
+  <si>
+    <t>customer_product__dop</t>
+  </si>
+  <si>
+    <t>customer_product__serial_number</t>
+  </si>
+  <si>
+    <t>customer_product__imei1</t>
+  </si>
+  <si>
+    <t>customer_product__imei2</t>
+  </si>
+  <si>
+    <t>customer_product__popurl</t>
+  </si>
+  <si>
+    <t>customer_product__product_id</t>
+  </si>
+  <si>
+    <t>customer_product__mst_model_id</t>
+  </si>
+  <si>
+    <t>problems__id</t>
+  </si>
+  <si>
+    <t>problems__remark</t>
+  </si>
+  <si>
+    <t>Bishnu</t>
+  </si>
+  <si>
+    <t>Das</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>somit.gate@gmail.com</t>
+  </si>
+  <si>
+    <t>flat no 123</t>
+  </si>
+  <si>
+    <t>apartment name</t>
+  </si>
+  <si>
+    <t>street name</t>
+  </si>
+  <si>
+    <t>near landmark</t>
+  </si>
+  <si>
+    <t>area name</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>2025-11-19T18:09:33.295174Z</t>
+  </si>
+  <si>
+    <t>5544598687485620</t>
+  </si>
+  <si>
+    <t>2025-11-19T18:09:33.296578Z</t>
+  </si>
+  <si>
+    <t>battery issue</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t>5644598687486620</t>
+  </si>
+  <si>
+    <t>Trisha</t>
+  </si>
+  <si>
+    <t>5744598687487620</t>
+  </si>
+  <si>
+    <t>Kajal</t>
+  </si>
+  <si>
+    <t>Kumari</t>
+  </si>
+  <si>
+    <t>5844598687488620</t>
+  </si>
+  <si>
+    <t>Anil</t>
+  </si>
+  <si>
+    <t>Thapa</t>
+  </si>
+  <si>
+    <t>5944598687489620</t>
   </si>
 </sst>
 </file>
@@ -54,13 +214,19 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -517,156 +683,161 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,44 +1159,44 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.6617647058824" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="16384" width="24.6617647058824" style="1"/>
+    <col min="1" max="16384" width="24.6617647058824" style="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="18" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="18" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" ht="18" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1033,4 +1204,529 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AA6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.94117647058824" defaultRowHeight="17.6" outlineLevelRow="5"/>
+  <cols>
+    <col min="1" max="1" width="19.9411764705882" customWidth="1"/>
+    <col min="2" max="2" width="13.6470588235294" customWidth="1"/>
+    <col min="3" max="3" width="19.7647058823529" customWidth="1"/>
+    <col min="4" max="4" width="10.4705882352941" customWidth="1"/>
+    <col min="5" max="5" width="18.4117647058824" customWidth="1"/>
+    <col min="6" max="6" width="18.2941176470588" customWidth="1"/>
+    <col min="7" max="7" width="22.6470588235294" customWidth="1"/>
+    <col min="8" max="8" width="25.4705882352941" customWidth="1"/>
+    <col min="9" max="9" width="18.9411764705882" customWidth="1"/>
+    <col min="10" max="10" width="19.5294117647059" style="2" customWidth="1"/>
+    <col min="11" max="11" width="27.1176470588235" customWidth="1"/>
+    <col min="12" max="12" width="31.2352941176471" customWidth="1"/>
+    <col min="13" max="13" width="27.4705882352941" customWidth="1"/>
+    <col min="14" max="14" width="25" customWidth="1"/>
+    <col min="15" max="15" width="20.9411764705882" customWidth="1"/>
+    <col min="16" max="16" width="24.0588235294118" customWidth="1"/>
+    <col min="17" max="17" width="23.5882352941176" customWidth="1"/>
+    <col min="18" max="18" width="21.4705882352941" customWidth="1"/>
+    <col min="19" max="19" width="26.3529411764706" customWidth="1"/>
+    <col min="20" max="20" width="30.5147058823529" customWidth="1"/>
+    <col min="21" max="22" width="21.6470588235294" customWidth="1"/>
+    <col min="23" max="23" width="26.3529411764706" customWidth="1"/>
+    <col min="24" max="24" width="26.1176470588235" customWidth="1"/>
+    <col min="25" max="25" width="28.7058823529412" customWidth="1"/>
+    <col min="26" max="26" width="11.5294117647059" customWidth="1"/>
+    <col min="27" max="27" width="15.6470588235294" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="16.8" spans="1:27">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="16.8" spans="1:27">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="1">
+        <v>412101</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="16.8" spans="1:27">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="1">
+        <v>412101</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="16.8" spans="1:27">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="1">
+        <v>412101</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="16.8" spans="1:27">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="1">
+        <v>412101</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="16.8" spans="1:27">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="1">
+        <v>412101</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>